<commit_message>
Template was updated, two additional cols were added.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ExcelReaderConsole\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocumentsMover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF18E1B4-F245-4E19-921C-0AD970FF5BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE00B7CE-747F-47A3-BD3B-17F462D757C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34305" yWindow="7485" windowWidth="20820" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="-120" windowWidth="27990" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$3:$BR$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$3:$BT$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
   <si>
     <t>Наименование (обязательный)</t>
   </si>
@@ -493,6 +493,18 @@
   </si>
   <si>
     <t>7860:</t>
+  </si>
+  <si>
+    <t>Текстовый PDF</t>
+  </si>
+  <si>
+    <t>Вложения</t>
+  </si>
+  <si>
+    <t>textpdf.txt</t>
+  </si>
+  <si>
+    <t>attach.txt; attach2.txt</t>
   </si>
 </sst>
 </file>
@@ -974,11 +986,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BM8"/>
+  <dimension ref="A1:BO8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,30 +998,31 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="9.140625" style="1"/>
-    <col min="23" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="33" width="9.140625" style="1"/>
-    <col min="34" max="37" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="41" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="45" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="51" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="56" width="9.140625" style="1"/>
-    <col min="57" max="61" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="65" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="9.140625" style="1"/>
+    <col min="25" max="26" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="35" width="9.140625" style="1"/>
+    <col min="36" max="39" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="43" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="47" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="53" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="58" width="9.140625" style="1"/>
+    <col min="59" max="63" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="67" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="68" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="22" t="s">
         <v>147</v>
@@ -1017,220 +1030,222 @@
       <c r="C1" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="P1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AK1" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="AJ1" s="19" t="s">
+      <c r="AL1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="AK1" s="19" t="s">
+      <c r="AM1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" s="19" t="s">
+      <c r="AN1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" s="19" t="s">
+      <c r="AO1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="AN1" s="19" t="s">
+      <c r="AP1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="AO1" s="19" t="s">
+      <c r="AQ1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="AP1" s="19" t="s">
+      <c r="AR1" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="AQ1" s="19" t="s">
+      <c r="AS1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="AR1" s="19" t="s">
+      <c r="AT1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="AS1" s="19" t="s">
+      <c r="AU1" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="AT1" s="19" t="s">
+      <c r="AV1" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="AU1" s="19" t="s">
+      <c r="AW1" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="AV1" s="19" t="s">
+      <c r="AX1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="AW1" s="19" t="s">
+      <c r="AY1" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="AX1" s="19" t="s">
+      <c r="AZ1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AY1" s="19" t="s">
+      <c r="BA1" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="AZ1" s="19" t="s">
+      <c r="BB1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="BA1" s="19" t="s">
+      <c r="BC1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="BB1" s="19" t="s">
+      <c r="BD1" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="BC1" s="19" t="s">
+      <c r="BE1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="BD1" s="19" t="s">
+      <c r="BF1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="BE1" s="19" t="s">
+      <c r="BG1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="BF1" s="19" t="s">
+      <c r="BH1" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="BG1" s="19" t="s">
+      <c r="BI1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="BH1" s="19" t="s">
+      <c r="BJ1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="BI1" s="19" t="s">
+      <c r="BK1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="BJ1" s="19" t="s">
+      <c r="BL1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="BK1" s="19" t="s">
+      <c r="BM1" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="BL1" s="19" t="s">
+      <c r="BN1" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="BM1" s="19" t="s">
+      <c r="BO1" s="19" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:65" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:67" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>8</v>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>17</v>
@@ -1241,23 +1256,23 @@
       <c r="N2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="U2" s="10" t="s">
         <v>8</v>
@@ -1287,10 +1302,10 @@
         <v>8</v>
       </c>
       <c r="AD2" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>4</v>
@@ -1317,10 +1332,10 @@
         <v>4</v>
       </c>
       <c r="AN2" s="10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="AO2" s="10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="AP2" s="10" t="s">
         <v>17</v>
@@ -1347,10 +1362,10 @@
         <v>17</v>
       </c>
       <c r="AX2" s="10" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="AY2" s="10" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="AZ2" s="10" t="s">
         <v>8</v>
@@ -1365,10 +1380,10 @@
         <v>8</v>
       </c>
       <c r="BD2" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="BE2" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="BF2" s="10" t="s">
         <v>4</v>
@@ -1380,10 +1395,10 @@
         <v>4</v>
       </c>
       <c r="BI2" s="10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="BJ2" s="10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="BK2" s="10" t="s">
         <v>17</v>
@@ -1394,227 +1409,241 @@
       <c r="BM2" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="BN2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO2" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:65" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:67" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="W3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AB3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AD3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AE3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AD3" s="7" t="s">
+      <c r="AF3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AE3" s="7" t="s">
+      <c r="AG3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AF3" s="7" t="s">
+      <c r="AH3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AG3" s="7" t="s">
+      <c r="AI3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AH3" s="7" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AI3" s="7" t="s">
+      <c r="AK3" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AJ3" s="7" t="s">
+      <c r="AL3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AK3" s="7" t="s">
+      <c r="AM3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AL3" s="7" t="s">
+      <c r="AN3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="AM3" s="7" t="s">
+      <c r="AO3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AN3" s="7" t="s">
+      <c r="AP3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="AO3" s="7" t="s">
+      <c r="AQ3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="AP3" s="7" t="s">
+      <c r="AR3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="AQ3" s="7" t="s">
+      <c r="AS3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="AR3" s="7" t="s">
+      <c r="AT3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="AS3" s="7" t="s">
+      <c r="AU3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="AT3" s="7" t="s">
+      <c r="AV3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="AU3" s="7" t="s">
+      <c r="AW3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="AV3" s="7" t="s">
+      <c r="AX3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="AW3" s="7" t="s">
+      <c r="AY3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AX3" s="7" t="s">
+      <c r="AZ3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AY3" s="7" t="s">
+      <c r="BA3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AZ3" s="7" t="s">
+      <c r="BB3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="BA3" s="7" t="s">
+      <c r="BC3" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="BB3" s="7" t="s">
+      <c r="BD3" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="BC3" s="7" t="s">
+      <c r="BE3" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="BD3" s="7" t="s">
+      <c r="BF3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="BE3" s="7" t="s">
+      <c r="BG3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="BF3" s="7" t="s">
+      <c r="BH3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="BG3" s="7" t="s">
+      <c r="BI3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="BH3" s="7" t="s">
+      <c r="BJ3" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="BI3" s="7" t="s">
+      <c r="BK3" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="BJ3" s="7" t="s">
+      <c r="BL3" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="BK3" s="7" t="s">
+      <c r="BM3" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="BL3" s="7" t="s">
+      <c r="BN3" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="BM3" s="7" t="s">
+      <c r="BO3" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:65" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:65" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1624,108 +1653,108 @@
       <c r="C5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="F5" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="M5" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:65" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="F6" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:65" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="I7" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="M7" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:65" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:BR3" xr:uid="{20F3A727-4776-4F8D-A07D-8A164782E8A8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:BR8">
+  <autoFilter ref="A3:BT3" xr:uid="{20F3A727-4776-4F8D-A07D-8A164782E8A8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:BT8">
       <sortCondition ref="A3"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="D1:BM3">
-    <sortCondition ref="D3:BM3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="F1:BO3">
+    <sortCondition ref="F3:BO3"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>